<commit_message>
seconds before disaster ...
</commit_message>
<xml_diff>
--- a/data/btaurus_blg_trypsin.xlsx
+++ b/data/btaurus_blg_trypsin.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
   <si>
     <t>peptide</t>
   </si>
@@ -95,24 +95,81 @@
     <t>19</t>
   </si>
   <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
     <t>K</t>
   </si>
   <si>
+    <t>R</t>
+  </si>
+  <si>
     <t>MK</t>
   </si>
   <si>
     <t>TK</t>
   </si>
   <si>
+    <t>TR</t>
+  </si>
+  <si>
+    <t>SR</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
     <t>FDK</t>
   </si>
   <si>
     <t>ALK</t>
   </si>
   <si>
+    <t>GHR</t>
+  </si>
+  <si>
+    <t>TSK</t>
+  </si>
+  <si>
     <t>IIAEK</t>
   </si>
   <si>
+    <t>RPNFK</t>
+  </si>
+  <si>
     <t>GLDIQK</t>
   </si>
   <si>
@@ -125,7 +182,10 @@
     <t>IDALNENK</t>
   </si>
   <si>
-    <t>WENGECAQK</t>
+    <t>SPCHLDPR</t>
+  </si>
+  <si>
+    <t>WWNGECAQK</t>
   </si>
   <si>
     <t>VLVLDTDYK</t>
@@ -134,16 +194,22 @@
     <t>TPEVDDEALEK</t>
   </si>
   <si>
-    <t>LSFNPTQLEEQCHI</t>
+    <t>SEPEGQVVQSR</t>
   </si>
   <si>
     <t>VYVEELKPTPEGDLEILLQK</t>
   </si>
   <si>
+    <t>LSFNPTQLEATHTWSPQLTPK</t>
+  </si>
+  <si>
+    <t>LALDMSVFPVALGASQGTGQR</t>
+  </si>
+  <si>
     <t>CLLLALALTCGAQALIVTQTMK</t>
   </si>
   <si>
-    <t>YLLFCMENSAEPEQSLVCQCLVR</t>
+    <t>YLLFCMENSAEPEQSLACQCLVR</t>
   </si>
   <si>
     <t>VAGTWYSLAMAASDISLLDAQSAPLR</t>
@@ -229,7 +295,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="C2" t="n">
         <v>86.0</v>
@@ -258,7 +324,7 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="C3" t="n">
         <v>117.0</v>
@@ -287,28 +353,28 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C4" t="n">
+        <v>198.0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>198.0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>175.119</v>
+      </c>
+      <c r="G4" t="n">
+        <v>88.063</v>
+      </c>
+      <c r="H4" t="n">
+        <v>59.045</v>
+      </c>
+      <c r="I4" t="n">
         <v>1.0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>278.153</v>
-      </c>
-      <c r="G4" t="n">
-        <v>139.58</v>
-      </c>
-      <c r="H4" t="n">
-        <v>93.389</v>
-      </c>
-      <c r="I4" t="n">
-        <v>2.0</v>
       </c>
     </row>
     <row r="5">
@@ -316,25 +382,25 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C5" t="n">
-        <v>92.0</v>
+        <v>1.0</v>
       </c>
       <c r="D5" t="n">
-        <v>93.0</v>
+        <v>2.0</v>
       </c>
       <c r="E5" t="n">
         <v>0.0</v>
       </c>
       <c r="F5" t="n">
-        <v>248.16</v>
+        <v>278.153</v>
       </c>
       <c r="G5" t="n">
-        <v>124.584</v>
+        <v>139.58</v>
       </c>
       <c r="H5" t="n">
-        <v>83.392</v>
+        <v>93.389</v>
       </c>
       <c r="I5" t="n">
         <v>2.0</v>
@@ -345,28 +411,28 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="C6" t="n">
-        <v>152.0</v>
+        <v>92.0</v>
       </c>
       <c r="D6" t="n">
-        <v>154.0</v>
+        <v>93.0</v>
       </c>
       <c r="E6" t="n">
         <v>0.0</v>
       </c>
       <c r="F6" t="n">
-        <v>409.208</v>
+        <v>248.16</v>
       </c>
       <c r="G6" t="n">
-        <v>205.108</v>
+        <v>124.584</v>
       </c>
       <c r="H6" t="n">
-        <v>137.074</v>
+        <v>83.392</v>
       </c>
       <c r="I6" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="7">
@@ -374,28 +440,28 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C7" t="n">
-        <v>155.0</v>
+        <v>186.0</v>
       </c>
       <c r="D7" t="n">
-        <v>157.0</v>
+        <v>187.0</v>
       </c>
       <c r="E7" t="n">
         <v>0.0</v>
       </c>
       <c r="F7" t="n">
-        <v>331.234</v>
+        <v>276.167</v>
       </c>
       <c r="G7" t="n">
-        <v>166.121</v>
+        <v>138.587</v>
       </c>
       <c r="H7" t="n">
-        <v>111.083</v>
+        <v>92.727</v>
       </c>
       <c r="I7" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="8">
@@ -403,28 +469,28 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="C8" t="n">
-        <v>87.0</v>
+        <v>188.0</v>
       </c>
       <c r="D8" t="n">
-        <v>91.0</v>
+        <v>189.0</v>
       </c>
       <c r="E8" t="n">
         <v>0.0</v>
       </c>
       <c r="F8" t="n">
-        <v>573.361</v>
+        <v>262.151</v>
       </c>
       <c r="G8" t="n">
-        <v>287.184</v>
+        <v>131.579</v>
       </c>
       <c r="H8" t="n">
-        <v>191.792</v>
+        <v>88.055</v>
       </c>
       <c r="I8" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="9">
@@ -432,28 +498,28 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="C9" t="n">
-        <v>25.0</v>
+        <v>202.0</v>
       </c>
       <c r="D9" t="n">
-        <v>30.0</v>
+        <v>203.0</v>
       </c>
       <c r="E9" t="n">
         <v>0.0</v>
       </c>
       <c r="F9" t="n">
-        <v>673.388</v>
+        <v>246.156</v>
       </c>
       <c r="G9" t="n">
-        <v>337.198</v>
+        <v>123.582</v>
       </c>
       <c r="H9" t="n">
-        <v>225.134</v>
+        <v>82.724</v>
       </c>
       <c r="I9" t="n">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="10">
@@ -461,28 +527,28 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C10" t="n">
-        <v>94.0</v>
+        <v>244.0</v>
       </c>
       <c r="D10" t="n">
-        <v>99.0</v>
+        <v>245.0</v>
       </c>
       <c r="E10" t="n">
         <v>0.0</v>
       </c>
       <c r="F10" t="n">
-        <v>674.424</v>
+        <v>203.139</v>
       </c>
       <c r="G10" t="n">
-        <v>337.715</v>
+        <v>102.073</v>
       </c>
       <c r="H10" t="n">
-        <v>225.479</v>
+        <v>68.385</v>
       </c>
       <c r="I10" t="n">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="11">
@@ -490,28 +556,28 @@
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C11" t="n">
-        <v>158.0</v>
+        <v>152.0</v>
       </c>
       <c r="D11" t="n">
-        <v>164.0</v>
+        <v>154.0</v>
       </c>
       <c r="E11" t="n">
         <v>0.0</v>
       </c>
       <c r="F11" t="n">
-        <v>837.476</v>
+        <v>409.208</v>
       </c>
       <c r="G11" t="n">
-        <v>419.242</v>
+        <v>205.108</v>
       </c>
       <c r="H11" t="n">
-        <v>279.83</v>
+        <v>137.074</v>
       </c>
       <c r="I11" t="n">
-        <v>7.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="12">
@@ -519,28 +585,28 @@
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="C12" t="n">
-        <v>100.0</v>
+        <v>155.0</v>
       </c>
       <c r="D12" t="n">
-        <v>107.0</v>
+        <v>157.0</v>
       </c>
       <c r="E12" t="n">
         <v>0.0</v>
       </c>
       <c r="F12" t="n">
-        <v>916.473</v>
+        <v>331.234</v>
       </c>
       <c r="G12" t="n">
-        <v>458.74</v>
+        <v>166.121</v>
       </c>
       <c r="H12" t="n">
-        <v>306.163</v>
+        <v>111.083</v>
       </c>
       <c r="I12" t="n">
-        <v>8.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="13">
@@ -548,28 +614,28 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="C13" t="n">
-        <v>77.0</v>
+        <v>199.0</v>
       </c>
       <c r="D13" t="n">
-        <v>85.0</v>
+        <v>201.0</v>
       </c>
       <c r="E13" t="n">
         <v>0.0</v>
       </c>
       <c r="F13" t="n">
-        <v>1121.468</v>
+        <v>369.199</v>
       </c>
       <c r="G13" t="n">
-        <v>561.238</v>
+        <v>185.103</v>
       </c>
       <c r="H13" t="n">
-        <v>374.494</v>
+        <v>123.738</v>
       </c>
       <c r="I13" t="n">
-        <v>9.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="14">
@@ -577,28 +643,28 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C14" t="n">
-        <v>108.0</v>
+        <v>241.0</v>
       </c>
       <c r="D14" t="n">
-        <v>116.0</v>
+        <v>243.0</v>
       </c>
       <c r="E14" t="n">
         <v>0.0</v>
       </c>
       <c r="F14" t="n">
-        <v>1065.583</v>
+        <v>335.193</v>
       </c>
       <c r="G14" t="n">
-        <v>533.295</v>
+        <v>168.1</v>
       </c>
       <c r="H14" t="n">
-        <v>355.866</v>
+        <v>112.402</v>
       </c>
       <c r="I14" t="n">
-        <v>9.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="15">
@@ -606,28 +672,28 @@
         <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="C15" t="n">
-        <v>141.0</v>
+        <v>87.0</v>
       </c>
       <c r="D15" t="n">
-        <v>151.0</v>
+        <v>91.0</v>
       </c>
       <c r="E15" t="n">
         <v>0.0</v>
       </c>
       <c r="F15" t="n">
-        <v>1245.585</v>
+        <v>573.361</v>
       </c>
       <c r="G15" t="n">
-        <v>623.296</v>
+        <v>287.184</v>
       </c>
       <c r="H15" t="n">
-        <v>415.866</v>
+        <v>191.792</v>
       </c>
       <c r="I15" t="n">
-        <v>11.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="16">
@@ -635,28 +701,28 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="C16" t="n">
-        <v>165.0</v>
+        <v>236.0</v>
       </c>
       <c r="D16" t="n">
-        <v>178.0</v>
+        <v>240.0</v>
       </c>
       <c r="E16" t="n">
         <v>0.0</v>
       </c>
       <c r="F16" t="n">
-        <v>1715.806</v>
+        <v>661.378</v>
       </c>
       <c r="G16" t="n">
-        <v>858.407</v>
+        <v>331.193</v>
       </c>
       <c r="H16" t="n">
-        <v>572.607</v>
+        <v>221.131</v>
       </c>
       <c r="I16" t="n">
-        <v>14.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="17">
@@ -664,28 +730,28 @@
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="C17" t="n">
-        <v>57.0</v>
+        <v>25.0</v>
       </c>
       <c r="D17" t="n">
-        <v>76.0</v>
+        <v>30.0</v>
       </c>
       <c r="E17" t="n">
         <v>0.0</v>
       </c>
       <c r="F17" t="n">
-        <v>2313.259</v>
+        <v>673.388</v>
       </c>
       <c r="G17" t="n">
-        <v>1157.133</v>
+        <v>337.198</v>
       </c>
       <c r="H17" t="n">
-        <v>771.758</v>
+        <v>225.134</v>
       </c>
       <c r="I17" t="n">
-        <v>20.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="18">
@@ -693,28 +759,28 @@
         <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C18" t="n">
-        <v>3.0</v>
+        <v>94.0</v>
       </c>
       <c r="D18" t="n">
-        <v>24.0</v>
+        <v>99.0</v>
       </c>
       <c r="E18" t="n">
         <v>0.0</v>
       </c>
       <c r="F18" t="n">
-        <v>2389.302</v>
+        <v>674.424</v>
       </c>
       <c r="G18" t="n">
-        <v>1195.154</v>
+        <v>337.715</v>
       </c>
       <c r="H18" t="n">
-        <v>797.105</v>
+        <v>225.479</v>
       </c>
       <c r="I18" t="n">
-        <v>22.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="19">
@@ -722,28 +788,28 @@
         <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="C19" t="n">
-        <v>118.0</v>
+        <v>158.0</v>
       </c>
       <c r="D19" t="n">
-        <v>140.0</v>
+        <v>164.0</v>
       </c>
       <c r="E19" t="n">
         <v>0.0</v>
       </c>
       <c r="F19" t="n">
-        <v>2846.298</v>
+        <v>837.476</v>
       </c>
       <c r="G19" t="n">
-        <v>1423.653</v>
+        <v>419.242</v>
       </c>
       <c r="H19" t="n">
-        <v>949.438</v>
+        <v>279.83</v>
       </c>
       <c r="I19" t="n">
-        <v>23.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="20">
@@ -751,27 +817,346 @@
         <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="C20" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>107.0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>916.473</v>
+      </c>
+      <c r="G20" t="n">
+        <v>458.74</v>
+      </c>
+      <c r="H20" t="n">
+        <v>306.163</v>
+      </c>
+      <c r="I20" t="n">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" t="n">
+        <v>190.0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>197.0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F21" t="n">
+        <v>981.457</v>
+      </c>
+      <c r="G21" t="n">
+        <v>491.232</v>
+      </c>
+      <c r="H21" t="n">
+        <v>327.824</v>
+      </c>
+      <c r="I21" t="n">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" t="n">
+        <v>77.0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>85.0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1178.505</v>
+      </c>
+      <c r="G22" t="n">
+        <v>589.756</v>
+      </c>
+      <c r="H22" t="n">
+        <v>393.506</v>
+      </c>
+      <c r="I22" t="n">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" t="n">
+        <v>108.0</v>
+      </c>
+      <c r="D23" t="n">
+        <v>116.0</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F23" t="n">
+        <v>1065.583</v>
+      </c>
+      <c r="G23" t="n">
+        <v>533.295</v>
+      </c>
+      <c r="H23" t="n">
+        <v>355.866</v>
+      </c>
+      <c r="I23" t="n">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" t="n">
+        <v>141.0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>151.0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>1245.585</v>
+      </c>
+      <c r="G24" t="n">
+        <v>623.296</v>
+      </c>
+      <c r="H24" t="n">
+        <v>415.866</v>
+      </c>
+      <c r="I24" t="n">
+        <v>11.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" t="n">
+        <v>225.0</v>
+      </c>
+      <c r="D25" t="n">
+        <v>235.0</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F25" t="n">
+        <v>1215.596</v>
+      </c>
+      <c r="G25" t="n">
+        <v>608.302</v>
+      </c>
+      <c r="H25" t="n">
+        <v>405.87</v>
+      </c>
+      <c r="I25" t="n">
+        <v>11.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" t="n">
+        <v>57.0</v>
+      </c>
+      <c r="D26" t="n">
+        <v>76.0</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F26" t="n">
+        <v>2313.259</v>
+      </c>
+      <c r="G26" t="n">
+        <v>1157.133</v>
+      </c>
+      <c r="H26" t="n">
+        <v>771.758</v>
+      </c>
+      <c r="I26" t="n">
+        <v>20.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" t="n">
+        <v>165.0</v>
+      </c>
+      <c r="D27" t="n">
+        <v>185.0</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F27" t="n">
+        <v>2396.224</v>
+      </c>
+      <c r="G27" t="n">
+        <v>1198.616</v>
+      </c>
+      <c r="H27" t="n">
+        <v>799.413</v>
+      </c>
+      <c r="I27" t="n">
+        <v>21.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" t="n">
+        <v>204.0</v>
+      </c>
+      <c r="D28" t="n">
+        <v>224.0</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F28" t="n">
+        <v>2118.101</v>
+      </c>
+      <c r="G28" t="n">
+        <v>1059.554</v>
+      </c>
+      <c r="H28" t="n">
+        <v>706.705</v>
+      </c>
+      <c r="I28" t="n">
+        <v>21.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D29" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F29" t="n">
+        <v>2389.302</v>
+      </c>
+      <c r="G29" t="n">
+        <v>1195.154</v>
+      </c>
+      <c r="H29" t="n">
+        <v>797.105</v>
+      </c>
+      <c r="I29" t="n">
+        <v>22.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" t="n">
+        <v>118.0</v>
+      </c>
+      <c r="D30" t="n">
+        <v>140.0</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F30" t="n">
+        <v>2818.267</v>
+      </c>
+      <c r="G30" t="n">
+        <v>1409.637</v>
+      </c>
+      <c r="H30" t="n">
+        <v>940.094</v>
+      </c>
+      <c r="I30" t="n">
+        <v>23.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" t="n">
         <v>31.0</v>
       </c>
-      <c r="D20" t="n">
+      <c r="D31" t="n">
         <v>56.0</v>
       </c>
-      <c r="E20" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F20" t="n">
+      <c r="E31" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F31" t="n">
         <v>2707.376</v>
       </c>
-      <c r="G20" t="n">
+      <c r="G31" t="n">
         <v>1354.192</v>
       </c>
-      <c r="H20" t="n">
+      <c r="H31" t="n">
         <v>903.13</v>
       </c>
-      <c r="I20" t="n">
+      <c r="I31" t="n">
         <v>26.0</v>
       </c>
     </row>

</xml_diff>